<commit_message>
Splite file for each year
</commit_message>
<xml_diff>
--- a/version.0.5/students_data/2565.xlsx
+++ b/version.0.5/students_data/2565.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2565" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,341 +422,261 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Student ID</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Face Status</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710151</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710151</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>นางสาวกรณิการ์ เต้นลือ</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710154</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710154</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>นางสาวกิตติมา ดารา</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710157</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710157</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
           <t>นางสาวณิชาพัฒน์ ปฐมพรวิวัฒน์</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710167</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710167</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
           <t>นายอัครพนธ์ อุดมทรัพย์</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710169</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710169</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>นางสาวอัจฉรียา ทองมาก</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710235</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710235</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
           <t>นายธนชาติ เอื้อยอ่อง</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710238</t>
+        </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710238</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
           <t>นายศิวัช จำรูญศิริรุ่งโรจน์</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710680</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710680</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>นางสาวชุติมา สหพรอุดมการ</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710683</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710683</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
           <t>นางสาวณฐพร สุขเจริญพรกุล</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710728</t>
+        </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710728</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
           <t>นางสาวสุภัทรา เค้าสำราญ</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710729</t>
+        </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710729</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
           <t>นางสาวสุภีร์กิติ์ พันธุ์บุญปลูก</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710730</t>
+        </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710730</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
           <t>นางสาวอคัมย์สิริ ฉุยเนย</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710736</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710736</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>นางสาวอินทิรา ภู่ขำ</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710860</t>
+        </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710860</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>นายจิรสิน รุ่งเรืองด้วยบุญ</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710861</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710861</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
           <t>นายเจษฎาพร อมรจิตรเวชกุล</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710866</t>
+        </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710866</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
           <t>นายณัฐพล ปินะสา</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710867</t>
+        </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710867</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
           <t>นางสาวดวงพร โคตมี</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710868</t>
+        </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710868</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
           <t>นางสาวธมกร นันทเศรษฐสิริ</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710873</t>
+        </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710873</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
           <t>นายภูริภัทร ลิสอน</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 650710915</t>
+        </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 650710915</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
           <t>นางสาวรัตนาวดี เมตตา</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>